<commit_message>
now with study 1 almost done
</commit_message>
<xml_diff>
--- a/paper/Stimuli For Study.xlsx
+++ b/paper/Stimuli For Study.xlsx
@@ -108,19 +108,19 @@
     <t xml:space="preserve">    Shipping Cost</t>
   </si>
   <si>
-    <t xml:space="preserve">    Date Received Days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Date Received Ratios</t>
-  </si>
-  <si>
-    <t>Choice 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Choice 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Amount Paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Shipping Time Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Shipping Time Ratios</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Option 2</t>
   </si>
 </sst>
 </file>
@@ -175,12 +175,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,6 +186,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -495,7 +498,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,125 +522,125 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="7"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="2"/>
+      <c r="L1" s="7"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="F2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="I2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="4" t="s">
+      <c r="L2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="6" t="s">
         <v>33</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>11</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>9</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>12</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>4</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>6</v>
       </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>5</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>6</v>
       </c>
       <c r="M4" s="1"/>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>14</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>15</v>
       </c>
     </row>
@@ -645,38 +648,38 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M5" s="1"/>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -684,38 +687,38 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -740,57 +743,57 @@
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="6">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5">
         <v>-10</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>-11</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>-9</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>-12</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>-4</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>-6</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>-5</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>-6</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>-14</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <v>-15</v>
       </c>
     </row>
@@ -798,38 +801,38 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="5" t="s">
+      <c r="K10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O10" s="5" t="s">
+      <c r="N10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -837,38 +840,38 @@
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I11" s="5" t="s">
+      <c r="H11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="J11" s="1"/>
-      <c r="K11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L11" s="5" t="s">
+      <c r="K11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O11" s="5" t="s">
+      <c r="N11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -893,135 +896,135 @@
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>-14</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>-5</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>-11</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>-8</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>-8</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>-5</v>
       </c>
       <c r="J14" s="1"/>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>-9</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>-7</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="6">
+      <c r="N14" s="5">
         <v>-8</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="5">
         <v>-3</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="J15" s="1"/>
-      <c r="K15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="5" t="s">
+      <c r="K15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="M15" s="1"/>
-      <c r="N15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O15" s="5" t="s">
+      <c r="N15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="5" t="s">
+      <c r="H16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="J16" s="1"/>
-      <c r="K16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L16" s="5" t="s">
+      <c r="K16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="M16" s="1"/>
-      <c r="N16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="5" t="s">
+      <c r="N16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>